<commit_message>
updated uncovered mRNA region after de novo sequencing
</commit_message>
<xml_diff>
--- a/Result/LSS/assemble_mRNA_uncovered.xlsx
+++ b/Result/LSS/assemble_mRNA_uncovered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shangsilin/Desktop/Autumn 2025/mRNA_sequencing/Result/LSS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6B0C7D-9BD3-1444-8BB3-BE054A50FC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED74AEFF-F772-7E4A-B6A7-71C8DFD58B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -559,6 +559,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -572,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -597,6 +603,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1341"/>
   <sheetViews>
-    <sheetView topLeftCell="A181" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A210" sqref="A210:D211"/>
+    <sheetView tabSelected="1" topLeftCell="A1250" zoomScale="226" workbookViewId="0">
+      <selection activeCell="J1260" sqref="J1260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26073,162 +26080,162 @@
       </c>
     </row>
     <row r="1259" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1259" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1259">
+      <c r="A1259" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1259" s="22">
         <v>3557.6279618205099</v>
       </c>
-      <c r="C1259">
+      <c r="C1259" s="22">
         <v>1530.01</v>
       </c>
-      <c r="D1259">
+      <c r="D1259" s="22">
         <v>7.2355914409637396</v>
       </c>
-      <c r="E1259">
+      <c r="E1259" s="22">
         <v>1192</v>
       </c>
-      <c r="F1259" t="s">
+      <c r="F1259" s="22" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="1260" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1260" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1260">
+      <c r="A1260" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1260" s="22">
         <v>3886.6752134540002</v>
       </c>
-      <c r="C1260">
+      <c r="C1260" s="22">
         <v>3367.4</v>
       </c>
-      <c r="D1260">
+      <c r="D1260" s="22">
         <v>7.9790357585430103</v>
       </c>
-      <c r="E1260">
+      <c r="E1260" s="22">
         <v>1192</v>
       </c>
-      <c r="F1260" t="s">
+      <c r="F1260" s="22" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="1261" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1261" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1261">
+      <c r="A1261" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1261" s="22">
         <v>4215.7307122546699</v>
       </c>
-      <c r="C1261">
+      <c r="C1261" s="22">
         <v>6316.45</v>
       </c>
-      <c r="D1261">
+      <c r="D1261" s="22">
         <v>8.64011208372116</v>
       </c>
-      <c r="E1261">
+      <c r="E1261" s="22">
         <v>1192</v>
       </c>
-      <c r="F1261" t="s">
+      <c r="F1261" s="22" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="1262" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1262" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1262">
+      <c r="A1262" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1262" s="22">
         <v>4544.7869030178899</v>
       </c>
-      <c r="C1262">
+      <c r="C1262" s="22">
         <v>8282.27</v>
       </c>
-      <c r="D1262">
+      <c r="D1262" s="22">
         <v>9.2100474512259094</v>
       </c>
-      <c r="E1262">
+      <c r="E1262" s="22">
         <v>1192</v>
       </c>
-      <c r="F1262" t="s">
+      <c r="F1262" s="22" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="1263" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1263" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1263">
+      <c r="A1263" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1263" s="22">
         <v>4873.8374262331699</v>
       </c>
-      <c r="C1263">
+      <c r="C1263" s="22">
         <v>10973.36</v>
       </c>
-      <c r="D1263">
+      <c r="D1263" s="22">
         <v>9.7131263669014007</v>
       </c>
-      <c r="E1263">
+      <c r="E1263" s="22">
         <v>1192</v>
       </c>
-      <c r="F1263" t="s">
+      <c r="F1263" s="22" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="1264" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1264" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1264">
+      <c r="A1264" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1264" s="22">
         <v>5202.89401359985</v>
       </c>
-      <c r="C1264">
+      <c r="C1264" s="22">
         <v>11284.68</v>
       </c>
-      <c r="D1264">
+      <c r="D1264" s="22">
         <v>10.200648074913</v>
       </c>
-      <c r="E1264">
+      <c r="E1264" s="22">
         <v>1192</v>
       </c>
-      <c r="F1264" t="s">
+      <c r="F1264" s="22" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="1265" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1265" t="s">
+      <c r="A1265" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B1265">
+      <c r="B1265" s="22">
         <v>5531.9417602888398</v>
       </c>
-      <c r="C1265">
+      <c r="C1265" s="22">
         <v>12300.07</v>
       </c>
-      <c r="D1265">
+      <c r="D1265" s="22">
         <v>10.6153033252239</v>
       </c>
-      <c r="E1265">
+      <c r="E1265" s="22">
         <v>1192</v>
       </c>
-      <c r="F1265" t="s">
+      <c r="F1265" s="22" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="1266" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1266" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1266">
+      <c r="A1266" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1266" s="22">
         <v>5861.0017364330997</v>
       </c>
-      <c r="C1266">
+      <c r="C1266" s="22">
         <v>11915.51</v>
       </c>
-      <c r="D1266">
+      <c r="D1266" s="22">
         <v>11.0403955594381</v>
       </c>
-      <c r="E1266">
+      <c r="E1266" s="22">
         <v>1192</v>
       </c>
-      <c r="F1266" t="s">
+      <c r="F1266" s="22" t="s">
         <v>111</v>
       </c>
     </row>
@@ -27741,8 +27748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D5C0F4-AF56-D34C-8AD0-3E058F8D8D14}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView zoomScale="168" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="C1" zoomScale="280" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27805,7 +27812,7 @@
         <v>1688.2349999999999</v>
       </c>
       <c r="C5" s="7">
-        <f t="shared" ref="C5:C11" si="0">E5-B5</f>
+        <f>E5-B5</f>
         <v>-4.6639979098017648E-3</v>
       </c>
       <c r="D5" s="7"/>
@@ -27840,7 +27847,7 @@
         <v>1993.2763</v>
       </c>
       <c r="C6" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C5:C11" si="0">E6-B6</f>
         <v>-2.3567375999391516E-3</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -28201,8 +28208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3A74C3-13E7-9B4D-87D3-E5733A838787}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScale="163" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28438,8 +28445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FB15AA-160B-5F46-8AAC-AC712875A935}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView topLeftCell="A2" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29424,7 +29431,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="G40" sqref="C40:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30471,7 +30478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72C6B039-4850-2544-B90B-7640CEE2EBFC}">
   <dimension ref="A1:F1341"/>
   <sheetViews>
-    <sheetView topLeftCell="A1179" workbookViewId="0">
+    <sheetView topLeftCell="A1073" workbookViewId="0">
       <selection activeCell="I1206" sqref="I1206"/>
     </sheetView>
   </sheetViews>

</xml_diff>